<commit_message>
[NEW] 200 Samples Data
</commit_message>
<xml_diff>
--- a/data/simple.xlsx
+++ b/data/simple.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francisco/Git/sa-uta8-utaut/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B93CC893-1C05-424B-86DD-28AA9CE8DB37}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11A87F94-97DB-7C4E-A417-5BF7944C85A5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="75">
   <si>
     <t>Your experience with AI systems?</t>
   </si>
@@ -244,12 +244,15 @@
   <si>
     <t>Q37</t>
   </si>
+  <si>
+    <t>Concerns? It seems that clinicians are more concerned about their patients' privacy and information instead of career concerns.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -271,13 +274,33 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="8" tint="-0.249977111117893"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -292,16 +315,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -19341,18 +19379,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED717278-CE49-9849-AE12-DC753556550F}">
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="119.1640625" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="6"/>
+    <col min="2" max="2" width="130" style="6" customWidth="1"/>
+    <col min="3" max="4" width="10.83203125" style="6"/>
+    <col min="5" max="5" width="65" style="6" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>37</v>
       </c>
@@ -19360,31 +19402,37 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.15">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.15">
+      <c r="B2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="7"/>
+      <c r="E2" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.15">
-      <c r="A4" s="2" t="s">
+      <c r="D3" s="7"/>
+      <c r="E3" s="8"/>
+    </row>
+    <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.15">
+      <c r="B4" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>41</v>
       </c>
@@ -19392,7 +19440,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>42</v>
       </c>
@@ -19400,7 +19448,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>43</v>
       </c>
@@ -19408,7 +19456,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>44</v>
       </c>
@@ -19416,7 +19464,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>45</v>
       </c>
@@ -19424,7 +19472,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>46</v>
       </c>
@@ -19432,7 +19480,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="16" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>47</v>
       </c>
@@ -19440,7 +19488,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="16" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>48</v>
       </c>
@@ -19448,7 +19496,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="16" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>49</v>
       </c>
@@ -19456,7 +19504,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="16" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>50</v>
       </c>
@@ -19464,7 +19512,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="16" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>51</v>
       </c>
@@ -19472,7 +19520,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="16" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>52</v>
       </c>
@@ -19480,7 +19528,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="16" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>53</v>
       </c>
@@ -19488,7 +19536,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="16" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>54</v>
       </c>
@@ -19496,7 +19544,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="16" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>55</v>
       </c>
@@ -19504,7 +19552,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="16" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>56</v>
       </c>
@@ -19512,7 +19560,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="16" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>57</v>
       </c>
@@ -19520,7 +19568,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="16" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>58</v>
       </c>
@@ -19528,7 +19576,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="16" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>59</v>
       </c>
@@ -19536,7 +19584,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="16" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>60</v>
       </c>
@@ -19544,7 +19592,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="16" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>61</v>
       </c>
@@ -19552,7 +19600,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="16" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>62</v>
       </c>
@@ -19560,7 +19608,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="16" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>63</v>
       </c>
@@ -19568,7 +19616,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="16" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>64</v>
       </c>
@@ -19576,7 +19624,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="16" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>65</v>
       </c>
@@ -19584,7 +19632,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="16" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>66</v>
       </c>
@@ -19592,7 +19640,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="16" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>67</v>
       </c>
@@ -19600,31 +19648,31 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="16" x14ac:dyDescent="0.15">
-      <c r="A32" s="2" t="s">
+    <row r="32" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="16" x14ac:dyDescent="0.15">
-      <c r="A33" s="2" t="s">
+    <row r="33" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="16" x14ac:dyDescent="0.15">
-      <c r="A34" s="2" t="s">
+    <row r="34" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="16" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>71</v>
       </c>
@@ -19632,7 +19680,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="16" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>72</v>
       </c>
@@ -19640,7 +19688,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="16" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>73</v>
       </c>
@@ -19649,6 +19697,10 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
[ADD] New EFA Methods
</commit_message>
<xml_diff>
--- a/data/simple.xlsx
+++ b/data/simple.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francisco/Git/sa-uta8-utaut/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A3ACB29-EE35-2D44-ACC4-1B6F44072B2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DFE3757-4D2E-E548-9962-CEF604258EE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -343,6 +343,7 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -580,6 +581,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -604,7 +606,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -19646,14 +19647,14 @@
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28.33203125" style="6" customWidth="1"/>
     <col min="2" max="2" width="6.5" style="6" customWidth="1"/>
-    <col min="3" max="3" width="6.1640625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="5.5" style="6" customWidth="1"/>
     <col min="4" max="4" width="126.1640625" style="6" customWidth="1"/>
     <col min="5" max="5" width="11.6640625" style="24" customWidth="1"/>
     <col min="6" max="6" width="7.33203125" style="6" customWidth="1"/>
@@ -19678,8 +19679,8 @@
         <v>1</v>
       </c>
       <c r="E2" s="5"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="28" t="s">
+      <c r="F2" s="30"/>
+      <c r="G2" s="29" t="s">
         <v>83</v>
       </c>
     </row>
@@ -19691,8 +19692,8 @@
         <v>2</v>
       </c>
       <c r="E3" s="9"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="28"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="29"/>
     </row>
     <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="C4" s="8" t="s">
@@ -19702,8 +19703,8 @@
         <v>3</v>
       </c>
       <c r="E4" s="5"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="28" t="s">
+      <c r="F4" s="31"/>
+      <c r="G4" s="29" t="s">
         <v>74</v>
       </c>
     </row>
@@ -19715,8 +19716,8 @@
         <v>4</v>
       </c>
       <c r="E5" s="9"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="28"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="29"/>
     </row>
     <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="C6" s="7" t="s">
@@ -19726,8 +19727,8 @@
         <v>5</v>
       </c>
       <c r="E6" s="9"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="28" t="s">
+      <c r="F6" s="32"/>
+      <c r="G6" s="29" t="s">
         <v>84</v>
       </c>
     </row>
@@ -19739,8 +19740,8 @@
         <v>6</v>
       </c>
       <c r="E7" s="9"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="28"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="29"/>
     </row>
     <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="C8" s="7" t="s">
@@ -19750,8 +19751,8 @@
         <v>7</v>
       </c>
       <c r="E8" s="9"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="28" t="s">
+      <c r="F8" s="33"/>
+      <c r="G8" s="29" t="s">
         <v>89</v>
       </c>
     </row>
@@ -19766,8 +19767,8 @@
         <v>8</v>
       </c>
       <c r="E9" s="9"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="28"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="29"/>
     </row>
     <row r="10" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
@@ -19785,8 +19786,8 @@
       <c r="E10" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="F10" s="33"/>
-      <c r="G10" s="28" t="s">
+      <c r="F10" s="34"/>
+      <c r="G10" s="29" t="s">
         <v>85</v>
       </c>
     </row>
@@ -19806,8 +19807,8 @@
       <c r="E11" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="F11" s="33"/>
-      <c r="G11" s="28"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="29"/>
     </row>
     <row r="12" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
@@ -19825,8 +19826,8 @@
       <c r="E12" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="F12" s="34"/>
-      <c r="G12" s="28" t="s">
+      <c r="F12" s="35"/>
+      <c r="G12" s="29" t="s">
         <v>86</v>
       </c>
     </row>
@@ -19846,11 +19847,11 @@
       <c r="E13" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="F13" s="34"/>
-      <c r="G13" s="28"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="29"/>
     </row>
     <row r="14" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="35" t="s">
+      <c r="A14" s="27" t="s">
         <v>91</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -19865,13 +19866,13 @@
       <c r="E14" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="F14" s="27"/>
-      <c r="G14" s="28" t="s">
+      <c r="F14" s="28"/>
+      <c r="G14" s="29" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="35" t="s">
+      <c r="A15" s="27" t="s">
         <v>91</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -19886,11 +19887,11 @@
       <c r="E15" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="F15" s="27"/>
-      <c r="G15" s="28"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="29"/>
     </row>
     <row r="16" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="27" t="s">
         <v>91</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -19909,7 +19910,7 @@
       <c r="G16" s="13"/>
     </row>
     <row r="17" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="35" t="s">
+      <c r="A17" s="27" t="s">
         <v>91</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -19928,7 +19929,7 @@
       <c r="G17" s="13"/>
     </row>
     <row r="18" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="35" t="s">
+      <c r="A18" s="27" t="s">
         <v>91</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -20131,7 +20132,7 @@
         <v>27</v>
       </c>
       <c r="E28" s="17" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="F28" s="12"/>
       <c r="G28" s="13"/>
@@ -20156,7 +20157,7 @@
       <c r="G29" s="13"/>
     </row>
     <row r="30" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" s="35" t="s">
+      <c r="A30" s="27" t="s">
         <v>97</v>
       </c>
       <c r="B30" s="2" t="s">
@@ -20175,7 +20176,7 @@
       <c r="G30" s="13"/>
     </row>
     <row r="31" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="35" t="s">
+      <c r="A31" s="27" t="s">
         <v>97</v>
       </c>
       <c r="B31" s="2" t="s">
@@ -20194,7 +20195,7 @@
       <c r="G31" s="13"/>
     </row>
     <row r="32" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="35" t="s">
+      <c r="A32" s="27" t="s">
         <v>97</v>
       </c>
       <c r="B32" s="2" t="s">
@@ -20270,7 +20271,7 @@
       <c r="G35" s="13"/>
     </row>
     <row r="36" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A36" s="35" t="s">
+      <c r="A36" s="27" t="s">
         <v>99</v>
       </c>
       <c r="B36" s="2" t="s">

</xml_diff>

<commit_message>
[UPDATE] CFA Model 0
</commit_message>
<xml_diff>
--- a/data/simple.xlsx
+++ b/data/simple.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francisco/Git/sa-uta8-utaut/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD748BAC-0A54-6D40-84A7-E51D86F13AB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91F6B2CA-CD11-4643-9E62-705D1578EFF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="104">
   <si>
     <t>Your experience with AI systems?</t>
   </si>
@@ -266,9 +266,6 @@
     <t>PerfExp</t>
   </si>
   <si>
-    <t>Privacy</t>
-  </si>
-  <si>
     <t>Trust</t>
   </si>
   <si>
@@ -323,10 +320,19 @@
     <t>App Trust</t>
   </si>
   <si>
-    <t>Security</t>
+    <t>Attitude/IntUse</t>
   </si>
   <si>
-    <t>Attitude/IntUse</t>
+    <t>Security/Risk</t>
+  </si>
+  <si>
+    <t>Privacy/Risk</t>
+  </si>
+  <si>
+    <t>Risk</t>
+  </si>
+  <si>
+    <t>Attitude</t>
   </si>
 </sst>
 </file>
@@ -19647,7 +19653,7 @@
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19678,10 +19684,12 @@
       <c r="D2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="5"/>
+      <c r="E2" s="5" t="s">
+        <v>102</v>
+      </c>
       <c r="F2" s="30"/>
       <c r="G2" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -19691,7 +19699,9 @@
       <c r="D3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="9"/>
+      <c r="E3" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="F3" s="30"/>
       <c r="G3" s="29"/>
     </row>
@@ -19702,7 +19712,9 @@
       <c r="D4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="5"/>
+      <c r="E4" s="5" t="s">
+        <v>102</v>
+      </c>
       <c r="F4" s="31"/>
       <c r="G4" s="29" t="s">
         <v>74</v>
@@ -19715,7 +19727,9 @@
       <c r="D5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="9"/>
+      <c r="E5" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="F5" s="31"/>
       <c r="G5" s="29"/>
     </row>
@@ -19729,7 +19743,7 @@
       <c r="E6" s="9"/>
       <c r="F6" s="32"/>
       <c r="G6" s="29" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -19753,7 +19767,7 @@
       <c r="E8" s="9"/>
       <c r="F8" s="33"/>
       <c r="G8" s="29" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -19772,7 +19786,7 @@
     </row>
     <row r="10" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>37</v>
@@ -19788,12 +19802,12 @@
       </c>
       <c r="F10" s="34"/>
       <c r="G10" s="29" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>38</v>
@@ -19812,7 +19826,7 @@
     </row>
     <row r="12" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>39</v>
@@ -19828,12 +19842,12 @@
       </c>
       <c r="F12" s="35"/>
       <c r="G12" s="29" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>40</v>
@@ -19852,7 +19866,7 @@
     </row>
     <row r="14" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>41</v>
@@ -19868,12 +19882,12 @@
       </c>
       <c r="F14" s="28"/>
       <c r="G14" s="29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>42</v>
@@ -19892,7 +19906,7 @@
     </row>
     <row r="16" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>43</v>
@@ -19911,7 +19925,7 @@
     </row>
     <row r="17" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>44</v>
@@ -19930,7 +19944,7 @@
     </row>
     <row r="18" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>45</v>
@@ -19949,7 +19963,7 @@
     </row>
     <row r="19" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>46</v>
@@ -19968,7 +19982,7 @@
     </row>
     <row r="20" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>47</v>
@@ -19987,7 +20001,7 @@
     </row>
     <row r="21" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>48</v>
@@ -20006,7 +20020,7 @@
     </row>
     <row r="22" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>49</v>
@@ -20025,7 +20039,7 @@
     </row>
     <row r="23" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>50</v>
@@ -20044,7 +20058,7 @@
     </row>
     <row r="24" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>51</v>
@@ -20063,7 +20077,7 @@
     </row>
     <row r="25" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>52</v>
@@ -20082,7 +20096,7 @@
     </row>
     <row r="26" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>53</v>
@@ -20094,14 +20108,14 @@
         <v>25</v>
       </c>
       <c r="E26" s="17" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F26" s="12"/>
       <c r="G26" s="13"/>
     </row>
     <row r="27" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>54</v>
@@ -20113,14 +20127,14 @@
         <v>26</v>
       </c>
       <c r="E27" s="17" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F27" s="12"/>
       <c r="G27" s="13"/>
     </row>
     <row r="28" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>55</v>
@@ -20132,14 +20146,14 @@
         <v>27</v>
       </c>
       <c r="E28" s="17" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F28" s="12"/>
       <c r="G28" s="13"/>
     </row>
     <row r="29" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>56</v>
@@ -20151,14 +20165,14 @@
         <v>28</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F29" s="12"/>
       <c r="G29" s="13"/>
     </row>
     <row r="30" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>57</v>
@@ -20177,7 +20191,7 @@
     </row>
     <row r="31" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>58</v>
@@ -20196,7 +20210,7 @@
     </row>
     <row r="32" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>59</v>
@@ -20208,14 +20222,14 @@
         <v>31</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>81</v>
+        <v>101</v>
       </c>
       <c r="F32" s="12"/>
       <c r="G32" s="13"/>
     </row>
     <row r="33" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>60</v>
@@ -20227,14 +20241,14 @@
         <v>32</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>81</v>
+        <v>101</v>
       </c>
       <c r="F33" s="12"/>
       <c r="G33" s="13"/>
     </row>
     <row r="34" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>61</v>
@@ -20246,14 +20260,14 @@
         <v>33</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>81</v>
+        <v>101</v>
       </c>
       <c r="F34" s="12"/>
       <c r="G34" s="13"/>
     </row>
     <row r="35" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>62</v>
@@ -20265,14 +20279,14 @@
         <v>34</v>
       </c>
       <c r="E35" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F35" s="12"/>
       <c r="G35" s="13"/>
     </row>
     <row r="36" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>63</v>
@@ -20284,14 +20298,14 @@
         <v>35</v>
       </c>
       <c r="E36" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F36" s="12"/>
       <c r="G36" s="13"/>
     </row>
     <row r="37" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="24" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>64</v>
@@ -20303,7 +20317,7 @@
         <v>36</v>
       </c>
       <c r="E37" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F37" s="12"/>
       <c r="G37" s="13"/>

</xml_diff>